<commit_message>
Worked on surface tying
Looks good so far
</commit_message>
<xml_diff>
--- a/merged_join_results.xlsx
+++ b/merged_join_results.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="JOIN TESTS" sheetId="1" r:id="rId1"/>
+    <sheet name="MESH DIFF" sheetId="2" r:id="rId2"/>
+    <sheet name="SMALL TIE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Merged Join Tests</t>
   </si>
@@ -41,9 +43,6 @@
     <t xml:space="preserve">Corner weights averaged together before adding the corner weights from the midside nodes </t>
   </si>
   <si>
-    <t>Corner weights are weighted by 2 or 3 factors averaged together.  Two if the the sample point is projected on the edge in question lies further away than the edge mid point</t>
-  </si>
-  <si>
     <t>Attempt 6</t>
   </si>
   <si>
@@ -65,9 +64,6 @@
     <t>Matched mesh - Join consists of all "1 to 1" equations</t>
   </si>
   <si>
-    <t>Reference case</t>
-  </si>
-  <si>
     <t>Midside nodes factors by same method as corner nodes alone - This added additional weighting to the nearest corner node also.</t>
   </si>
   <si>
@@ -78,13 +74,184 @@
   </si>
   <si>
     <t>Just the corners used in the equations</t>
+  </si>
+  <si>
+    <t>Left block (master) is 6x4x4</t>
+  </si>
+  <si>
+    <t>Right block (slave) is 4x4x2</t>
+  </si>
+  <si>
+    <t>Small Test model - Master on left - no center line symmetry</t>
+  </si>
+  <si>
+    <t>Exploded view</t>
+  </si>
+  <si>
+    <t>Fixed on left face - applied traction on the right face</t>
+  </si>
+  <si>
+    <t>********************************************************************************</t>
+  </si>
+  <si>
+    <t>*SURFACE, NAME=ARB_AS, TYPE=ELEMENT</t>
+  </si>
+  <si>
+    <t>1, S6</t>
+  </si>
+  <si>
+    <t>2, S6</t>
+  </si>
+  <si>
+    <t>3, S6</t>
+  </si>
+  <si>
+    <t>4, S6</t>
+  </si>
+  <si>
+    <t>*SURFACE, NAME=ARB_BS, TYPE=ELEMENT</t>
+  </si>
+  <si>
+    <t>9, S3</t>
+  </si>
+  <si>
+    <t>10, S3</t>
+  </si>
+  <si>
+    <t>11, S3</t>
+  </si>
+  <si>
+    <t>15, S3</t>
+  </si>
+  <si>
+    <t>16, S3</t>
+  </si>
+  <si>
+    <t>17, S3</t>
+  </si>
+  <si>
+    <t>21, S3</t>
+  </si>
+  <si>
+    <t>22, S3</t>
+  </si>
+  <si>
+    <t>23, S3</t>
+  </si>
+  <si>
+    <t>*TIE</t>
+  </si>
+  <si>
+    <t>ARB_AS, ARB_BS</t>
+  </si>
+  <si>
+    <t>VonMises Stress</t>
+  </si>
+  <si>
+    <t>Displacements magnified 100x</t>
+  </si>
+  <si>
+    <t>Close look at interface…</t>
+  </si>
+  <si>
+    <t>Displacement Field - pretty squiggly at interface</t>
+  </si>
+  <si>
+    <t>I was afraid it was going to be slow but it does not seem so.</t>
+  </si>
+  <si>
+    <t>Here's the test case - looks pretty good and a lot simpler than writing all those "*EQUATION" cards and transformations</t>
+  </si>
+  <si>
+    <t>Same modal as above but hand edited to add the surfaces and ties - not a lot of coding</t>
+  </si>
+  <si>
+    <t>These are still separate meshes - just tied 1 to 1 at the interface</t>
+  </si>
+  <si>
+    <t>Numbers look pretty good compared to the case at the top where the nodes are all mapped 1 to 1.</t>
+  </si>
+  <si>
+    <t>Note: this method was first tested on a smaller model - the results are on the "SMALL TIE" tab of this workbook</t>
+  </si>
+  <si>
+    <t>Calculix execution time</t>
+  </si>
+  <si>
+    <t>RS6_X1</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>RS6_TIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attempt 0 - </t>
+  </si>
+  <si>
+    <t>ONE MESH MODEL - NO JOIN…</t>
+  </si>
+  <si>
+    <t>Reference cases</t>
+  </si>
+  <si>
+    <t>This model hand edited from 1 to 1 model shown to the left</t>
+  </si>
+  <si>
+    <t>Swapping which is the master and which is the slave got slightly better results</t>
+  </si>
+  <si>
+    <t>Here B is the slave and A is the master</t>
+  </si>
+  <si>
+    <t>ARB_BS, ARB_AS</t>
+  </si>
+  <si>
+    <t>Slave surface is listed first on the *TIE card</t>
+  </si>
+  <si>
+    <t>COOL</t>
+  </si>
+  <si>
+    <t>SWAPPING SLAVE AND MASTER…</t>
+  </si>
+  <si>
+    <t>MASTER Contact surface of the left side</t>
+  </si>
+  <si>
+    <t>SLAVE Contact surface of the right side</t>
+  </si>
+  <si>
+    <t>Looks much better</t>
+  </si>
+  <si>
+    <t>Lower stresses with minimal gapping - more linear join line</t>
+  </si>
+  <si>
+    <t>Corner weights are weighted by 2 or 3 factors averaged together.  Two if the  sample point is projected on the edge in question lies further away than the edge mid point</t>
+  </si>
+  <si>
+    <t>Learned you don't have to do nonlinear analysis to take advantage of Calculix/ABAQUS surface tying</t>
+  </si>
+  <si>
+    <t>Still some small displacement discontinuities - but a lot better than my brute force method.</t>
+  </si>
+  <si>
+    <t>Looking into Calculix Surface Tying…</t>
+  </si>
+  <si>
+    <t>Note: similar behavior that I was getting with the *EQUATIONS in my JOIN TESTS</t>
+  </si>
+  <si>
+    <t>Displacement field is much better behaved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +267,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,14 +305,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,6 +687,1652 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>15552</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>101083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>387</xdr:row>
+      <xdr:rowOff>99036</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228532" y="65788593"/>
+          <a:ext cx="6927978" cy="6529382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>414326</xdr:colOff>
+      <xdr:row>389</xdr:row>
+      <xdr:rowOff>85823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9097347" y="65687510"/>
+          <a:ext cx="7085714" cy="6990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7776</xdr:colOff>
+      <xdr:row>388</xdr:row>
+      <xdr:rowOff>124408</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3226836" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1220756" y="72529959"/>
+          <a:ext cx="3226836" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>It ends up that the better method is actually faster </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- at least for small problems</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>606489</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>299705</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>31102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9703836" y="933061"/>
+          <a:ext cx="6971093" cy="6562531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>150327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>307133</xdr:colOff>
+      <xdr:row>384</xdr:row>
+      <xdr:rowOff>45358</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16709572" y="68158827"/>
+          <a:ext cx="6309394" cy="5038531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>********************************************************************************</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>*SURFACE, NAME=ARB_AS, TYPE=ELEMENT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>4, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>5, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>6, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>7, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>8, S6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>********************************************************************************</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>*SURFACE, NAME=ARB_BS, TYPE=ELEMENT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>33, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>34, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>41, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>42, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>49, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>50, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>57, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>58, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>65, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>66, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>73, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>74, S3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>********************************************************************************</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>*TIE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ARB_AS, ARB_BS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>********************************************************************************</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>31102</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>132183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>403251</xdr:colOff>
+      <xdr:row>438</xdr:row>
+      <xdr:rowOff>178837</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1244082" y="75539081"/>
+          <a:ext cx="7043536" cy="6391470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="5486400"/>
+          <a:ext cx="419100" cy="563880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800"/>
+            <a:t>B</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6461760" y="5273040"/>
+          <a:ext cx="419100" cy="563880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615940" y="4472940"/>
+          <a:ext cx="15240" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5349240" y="220980"/>
+          <a:ext cx="2766060" cy="632460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>In all models, the left side mesh (B) is the master - (except for a test case at the bottom of the sheet)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>399</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5920740" y="73136760"/>
+          <a:ext cx="7551420" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Using calculix notation (opposite of my slave/master designation) it looks like the more dense mesh should be the slave</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7421880" y="4991100"/>
+          <a:ext cx="15240" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3421380" y="5501640"/>
+          <a:ext cx="15240" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>426</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 27"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8778240" y="75849480"/>
+          <a:ext cx="3970020" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>FROM THE CALCULIX MANUAL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The dependent surface is called the slave surface, the independant-</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>dent surface is the master surface. The user can freely decide which surface he</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>takes as slave and which as master. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NOTE: DUMMY ME - The</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> nomenclature I adopted was just the opposite.  Theirs makes a lot more sense.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>596471</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>22861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="1097281"/>
+          <a:ext cx="7302070" cy="6972300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>182881</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>100302</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828801" y="1280160"/>
+          <a:ext cx="4450080" cy="2843502"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>578468</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>16806</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="1325880"/>
+          <a:ext cx="5219048" cy="2714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>56533</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>113943</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="5486400"/>
+          <a:ext cx="4933333" cy="2857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9195</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077201" y="9273541"/>
+          <a:ext cx="3514394" cy="2994660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>594361</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>548641</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>14547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3032761" y="9166860"/>
+          <a:ext cx="3611880" cy="3283527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>418438</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>127208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="17739360"/>
+          <a:ext cx="5295238" cy="3419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>411481</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>40457</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7696201" y="17975581"/>
+          <a:ext cx="6736080" cy="6022156"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>189638</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>31922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="25405080"/>
+          <a:ext cx="6895238" cy="3704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>270144</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>22861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9570720" y="25313641"/>
+          <a:ext cx="2891424" cy="6164580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>27733</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>79589</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="30906720"/>
+          <a:ext cx="6733333" cy="3371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="FF0000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>138498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1272540" y="35692080"/>
+          <a:ext cx="6080760" cy="5960178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>553466</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>70008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1363980" y="42519600"/>
+          <a:ext cx="7114286" cy="3819048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>418209</xdr:colOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>140472</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="47365920"/>
+          <a:ext cx="7123809" cy="3980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>18590</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>12350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="40965120"/>
+          <a:ext cx="3676190" cy="7876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1569720" y="51694080"/>
+          <a:ext cx="2712720" cy="472440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>THE SLAVE MESH (CALCULIX DEF)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> SHOULD BE THE MORE DENSE MESH</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -715,32 +2601,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P300"/>
+  <dimension ref="A2:V411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I342" sqref="I342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>12</v>
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="16:16" x14ac:dyDescent="0.3">
@@ -755,27 +2658,27 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172" spans="4:4" x14ac:dyDescent="0.3">
@@ -785,7 +2688,7 @@
     </row>
     <row r="212" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D212" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="213" spans="4:4" x14ac:dyDescent="0.3">
@@ -795,29 +2698,350 @@
     </row>
     <row r="258" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D258" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="259" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D259" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="299" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D299" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="300" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D300" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="342" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C342" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="343" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C343" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="345" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C345" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="348" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C348" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="350" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C350" t="s">
+        <v>47</v>
+      </c>
+      <c r="P350" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="352" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C352" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="393" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C393" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="394" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C394" t="s">
+        <v>50</v>
+      </c>
+      <c r="D394">
+        <v>0.62</v>
+      </c>
+      <c r="E394" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="395" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C395" t="s">
+        <v>52</v>
+      </c>
+      <c r="D395">
+        <v>0.41</v>
+      </c>
+      <c r="E395" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="401" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C401" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="402" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D402" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="403" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="404" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H404" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="406" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O406" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="408" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O408" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="409" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O409" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="410" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O410" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="411" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O411" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="P50" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:R257"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+      <c r="N49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J77" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J82" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J90" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J91" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J92" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N97" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>40</v>
+      </c>
+      <c r="G136" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B194" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H194" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="222" spans="18:18" x14ac:dyDescent="0.3">
+      <c r="R222" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C231" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D257" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating master/slave switch and begin *TIE coding
</commit_message>
<xml_diff>
--- a/merged_join_results.xlsx
+++ b/merged_join_results.xlsx
@@ -355,16 +355,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1384,16 +1384,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>399</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
       <xdr:row>402</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1402,14 +1402,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5920740" y="73136760"/>
-          <a:ext cx="7551420" cy="419100"/>
+          <a:off x="6225540" y="73075800"/>
+          <a:ext cx="3726180" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -1567,8 +1570,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>426</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:row>428</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1577,8 +1580,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8778240" y="75849480"/>
-          <a:ext cx="3970020" cy="2133600"/>
+          <a:off x="8778240" y="75864720"/>
+          <a:ext cx="3970020" cy="2567940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1655,7 +1658,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> nomenclature I adopted was just the opposite.  Theirs makes a lot more sense.</a:t>
+            <a:t> nomenclature I adopted was just the opposite.  Theirs makes a lot more sense. I changed my notation inside the code to agree with Calculix</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2603,22 +2606,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V411"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I342" sqref="I342"/>
+    <sheetView tabSelected="1" topLeftCell="A396" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O415" sqref="O415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
@@ -2788,7 +2791,7 @@
     </row>
     <row r="403" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="404" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H404" s="5" t="s">
+      <c r="H404" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>